<commit_message>
updated down data file
</commit_message>
<xml_diff>
--- a/protocols/data/TCGA-Ovarian-MesenvsImmuno_UP.xlsx
+++ b/protocols/data/TCGA-Ovarian-MesenvsImmuno_UP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinahanspers/Dropbox (Gladstone)/Work/github/cytoscape-tutorials/protocols/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FD71DEB-896F-6A47-BF02-AA0A1C2E79C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F19F30-55CD-4D4B-88AA-18877010555E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3260" windowWidth="27240" windowHeight="16440" xr2:uid="{26D9F7F8-A4DC-ED47-A1A3-1E9A09064A47}"/>
   </bookViews>
@@ -85,6 +85,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEA8F92"/>
+      <color rgb="FFFF9B9E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -396,7 +402,7 @@
   <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2541,7 +2547,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2551,6 +2557,40 @@
         <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF9B9E"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFEA8F92"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF9B9E"/>
+        <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>